<commit_message>
OSA03 rest of the filters
</commit_message>
<xml_diff>
--- a/InputFiles/ICDC/TC02_ICDC_TCL01_StudyType-Genomics.xlsx
+++ b/InputFiles/ICDC/TC02_ICDC_TCL01_StudyType-Genomics.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10714"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sohilz2/Automation/poc-07-15-2024/Commons_Automation/InputFiles/ICDC/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\epishinavv\git\Commons_Automation\InputFiles\ICDC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F069C395-C5FC-D74C-B745-5BBC64BAC4EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEE63341-01F6-477B-8A39-E701A1AD9C46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-47360" yWindow="-4940" windowWidth="42480" windowHeight="27840" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -60,20 +60,24 @@
     <t>CaseFilesTab</t>
   </si>
   <si>
+    <t>TC02_ICDC_TCL01_StudyType-Genomics_TSVData.xlsx</t>
+  </si>
+  <si>
     <t>TC02_ICDC_TCL01_StudyType-Genomics_WebData.xlsx</t>
   </si>
   <si>
-    <t>TC02_ICDC_TCL01_StudyType-Genomics_TSVData.xlsx</t>
-  </si>
-  <si>
     <t>SELECT
-    DISTINCT TRIM(c.case_record_id) AS "Case ID",
-    TRIM(st.clinical_study_designation) AS "Study Code",
-    TRIM(st.clinical_study_type) AS "Study Type",
+    DISTINCT c.case_record_id AS "Case ID",
+    st.clinical_study_designation AS "Study Code",
+    st.clinical_study_type AS "Study Type",
     dmg.breed AS "Breed",
     diag.disease_term AS "Diagnosis",
     diag.stage_of_disease AS "Stage Of Disease",
-    COALESCE(CAST(dmg.patient_age_at_enrollment AS INT), '') AS "Age", 
+    CASE 
+    WHEN dmg.patient_age_at_enrollment = CAST(dmg.patient_age_at_enrollment AS INT) 
+    THEN CAST(CAST(dmg.patient_age_at_enrollment AS INT) AS TEXT)
+    ELSE CAST(dmg.patient_age_at_enrollment AS TEXT)
+END AS "Age", 
     COALESCE(TRIM(dmg.sex), '') AS "Sex",   
     COALESCE(dmg.neutered_indicator, '') AS "Neutered Status",  
     COALESCE(
@@ -113,6 +117,35 @@
 LIMIT 100;</t>
   </si>
   <si>
+    <t>SELECT
+    COUNT(DISTINCT p.program_acronym) AS "Programs",
+    COUNT(DISTINCT st.clinical_study_designation) AS "Studies",
+    COUNT(DISTINCT c.case_record_id) AS "Cases",
+    COUNT(DISTINCT smp.sample_id) AS "Samples",
+    COUNT(DISTINCT cf.file_name) AS "Case Files",         
+    COUNT(DISTINCT sf.file_name) AS "Study Files" 
+FROM 
+    df_program p
+JOIN 
+    df_study st ON p.program_acronym = st."program.program_acronym"
+JOIN 
+    df_case c ON st.clinical_study_designation = c."study.clinical_study_designation"
+JOIN 
+    df_demographic dmg ON dmg."case.case_record_id" = c.case_record_id
+JOIN 
+    df_diagnosis diag ON diag."case.case_record_id" = c.case_record_id
+JOIN 
+    df_enrollment enr ON enr."case.case_record_id" = c.case_record_id
+JOIN 
+    df_sample smp ON smp."case.case_record_id" = c.case_record_id
+LEFT JOIN 
+    df_case_file cf ON cf."sample.sample_id" = smp.sample_id
+LEFT JOIN 
+    df_study_file sf ON sf."study.clinical_study_designation" = st.clinical_study_designation
+WHERE 
+    st.clinical_study_designation = 'TCL01' AND st.clinical_study_type = 'Genomics';</t>
+  </si>
+  <si>
     <t>SELECT DISTINCT
     smp.sample_id AS "Sample ID",
     c.case_record_id AS "Case ID",
@@ -124,7 +157,7 @@
     COALESCE(smp.tumor_grade, '') AS "Tumor Grade",
     COALESCE(smp.sample_chronology, '') AS "Sample Chronology",
     COALESCE(smp.percentage_tumor, '') AS "Percentage Tumor",
-    COALESCE(TRIM(smp.necropsy_sample), '') AS "Necropsy Sample",
+    COALESCE(smp.necropsy_sample, '') AS "Necropsy Sample",
     COALESCE(smp.sample_preservation, '') AS "Sample Preservation"
 FROM 
     df_sample smp
@@ -151,93 +184,6 @@
 ORDER BY 
     smp.sample_id ASC
 LIMIT 100;</t>
-  </si>
-  <si>
-    <t>SELECT DISTINCT
-    TRIM(sf.file_name) AS "File Name",
-    TRIM(sf.file_type) AS "File Type",
-    'study' AS "Association",
-    TRIM(sf.file_description) AS "Description",
-    CASE
-        WHEN sf.file_name LIKE '%.bai' THEN 'bai'
-        WHEN sf.file_name LIKE '%.bam' THEN 'bam'
-        WHEN sf.file_name LIKE '%.csv' THEN 'csv'
-        WHEN sf.file_name LIKE '%.doc' THEN 'doc'
-        WHEN sf.file_name LIKE '%.docx' THEN 'docx'
-        WHEN sf.file_name LIKE '%.gz' THEN 'gz'
-        WHEN sf.file_name LIKE '%.pdf' THEN 'pdf'
-        WHEN sf.file_name LIKE '%.rtf' THEN 'rtf'
-        WHEN sf.file_name LIKE '%.tbi' THEN 'tbi'
-        WHEN sf.file_name LIKE '%.tif' THEN 'tif'
-        WHEN sf.file_name LIKE '%.xls' THEN 'xls'
-        WHEN sf.file_name LIKE '%.xlsx' THEN 'xlsx'
-        ELSE 'Unknown'
-    END AS "Format",
-    CASE     
-        WHEN sf.file_size &gt;= 1024 * 1024 * 1024 THEN 
-            ROUND(sf.file_size / (1024.0 * 1024.0 * 1024.0), 2) || ' GB' 
-        WHEN sf.file_size &gt;= 1024 * 1024 THEN 
-            ROUND(sf.file_size / (1024.0 * 1024.0), 2) || ' MB' 
-        WHEN sf.file_size &gt;= 1024 THEN 
-            ROUND(sf.file_size / 1024.0, 2) || ' KB' 
-        ELSE 
-            ROUND(sf.file_size, 2) || ' Bytes' 
-    END AS "Size",
-    st.clinical_study_designation AS "Study Code"
-FROM 
-    df_case_file cf
-JOIN 
-    df_sample smp ON cf."sample.sample_id" = smp.sample_id
-JOIN 
-    df_case c ON smp."case.case_record_id" = c.case_record_id
-JOIN 
-    df_study st ON c."study.clinical_study_designation" = st.clinical_study_designation
-JOIN 
-    df_program p ON st."program.program_acronym" = p.program_acronym
-JOIN 
-    df_demographic dmg ON dmg."case.case_record_id" = c.case_record_id
-JOIN 
-    df_diagnosis diag ON diag."case.case_record_id" = c.case_record_id
-JOIN 
-    df_enrollment enr ON enr."case.case_record_id" = c.case_record_id
-JOIN 
-    df_publication pub ON pub."study.clinical_study_designation" = st.clinical_study_designation
-LEFT JOIN 
-    df_study_file sf ON sf."study.clinical_study_designation" = st.clinical_study_designation
-WHERE
-    st.clinical_study_designation = 'TCL01' AND st.clinical_study_type = 'Genomics'
-ORDER BY 
-    sf.file_name ASC
-LIMIT 100;</t>
-  </si>
-  <si>
-    <t>SELECT
-    COUNT(DISTINCT p.program_acronym) AS "Programs",
-    COUNT(DISTINCT st.clinical_study_designation) AS "Studies",
-    COUNT(DISTINCT c.case_record_id) AS "Cases",
-    COUNT(DISTINCT smp.sample_id) AS "Samples",
-    COUNT(DISTINCT cf.file_name) AS "Case Files",         
-    COUNT(DISTINCT sf.file_name) AS "Study Files" 
-FROM 
-    df_program p
-JOIN 
-    df_study st ON p.program_acronym = st."program.program_acronym"
-JOIN 
-    df_case c ON st.clinical_study_designation = c."study.clinical_study_designation"
-JOIN 
-    df_demographic dmg ON dmg."case.case_record_id" = c.case_record_id
-JOIN 
-    df_diagnosis diag ON diag."case.case_record_id" = c.case_record_id
-JOIN 
-    df_enrollment enr ON enr."case.case_record_id" = c.case_record_id
-JOIN 
-    df_sample smp ON smp."case.case_record_id" = c.case_record_id
-LEFT JOIN 
-    df_case_file cf ON cf."sample.sample_id" = smp.sample_id
-LEFT JOIN 
-    df_study_file sf ON sf."study.clinical_study_designation" = st.clinical_study_designation
-WHERE 
-    st.clinical_study_designation = 'TCL01' AND st.clinical_study_type = 'Genomics';</t>
   </si>
   <si>
     <t>SELECT 
@@ -316,35 +262,72 @@
     cf.file_name ASC
 LIMIT 100;</t>
   </si>
+  <si>
+    <t>SELECT DISTINCT
+    sf.file_name AS "File Name",
+    sf.file_type AS "File Type",
+    'study' AS "Association",
+    sf.file_description AS "Description",
+    CASE
+        WHEN sf.file_name LIKE '%.bai' THEN 'bai'
+        WHEN sf.file_name LIKE '%.bam' THEN 'bam'
+        WHEN sf.file_name LIKE '%.csv' THEN 'csv'
+        WHEN sf.file_name LIKE '%.doc' THEN 'doc'
+        WHEN sf.file_name LIKE '%.docx' THEN 'docx'
+        WHEN sf.file_name LIKE '%.gz' THEN 'gz'
+        WHEN sf.file_name LIKE '%.pdf' THEN 'pdf'
+        WHEN sf.file_name LIKE '%.rtf' THEN 'rtf'
+        WHEN sf.file_name LIKE '%.tbi' THEN 'tbi'
+        WHEN sf.file_name LIKE '%.tif' THEN 'tif'
+        WHEN sf.file_name LIKE '%.xls' THEN 'xls'
+        WHEN sf.file_name LIKE '%.xlsx' THEN 'xlsx'
+        ELSE 'Unknown'
+    END AS "Format",
+    CASE     
+        WHEN sf.file_size &gt;= 1024 * 1024 * 1024 THEN 
+            ROUND(sf.file_size / (1024.0 * 1024.0 * 1024.0), 2) || ' GB' 
+        WHEN sf.file_size &gt;= 1024 * 1024 THEN 
+            ROUND(sf.file_size / (1024.0 * 1024.0), 2) || ' MB' 
+        WHEN sf.file_size &gt;= 1024 THEN 
+            ROUND(sf.file_size / 1024.0, 2) || ' KB' 
+        ELSE 
+            ROUND(sf.file_size, 2) || ' Bytes' 
+    END AS "Size",
+    st.clinical_study_designation AS "Study Code"
+FROM 
+    df_case_file cf
+JOIN 
+    df_sample smp ON cf."sample.sample_id" = smp.sample_id
+JOIN 
+    df_case c ON smp."case.case_record_id" = c.case_record_id
+JOIN 
+    df_study st ON c."study.clinical_study_designation" = st.clinical_study_designation
+JOIN 
+    df_program p ON st."program.program_acronym" = p.program_acronym
+JOIN 
+    df_demographic dmg ON dmg."case.case_record_id" = c.case_record_id
+JOIN 
+    df_diagnosis diag ON diag."case.case_record_id" = c.case_record_id
+JOIN 
+    df_enrollment enr ON enr."case.case_record_id" = c.case_record_id
+JOIN 
+    df_publication pub ON pub."study.clinical_study_designation" = st.clinical_study_designation
+LEFT JOIN 
+    df_study_file sf ON sf."study.clinical_study_designation" = st.clinical_study_designation
+WHERE
+    st.clinical_study_designation = 'TCL01' AND st.clinical_study_type = 'Genomics'
+ORDER BY 
+    sf.file_name ASC
+LIMIT 100;</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -397,20 +380,11 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -736,19 +710,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C538400-E87C-4027-A918-A51DB80B3430}">
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="75.83203125" customWidth="1"/>
-    <col min="4" max="4" width="70.1640625" customWidth="1"/>
-    <col min="5" max="5" width="63.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="75.77734375" customWidth="1"/>
+    <col min="4" max="4" width="70.109375" customWidth="1"/>
+    <col min="5" max="5" width="63.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -765,55 +739,55 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>6</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="4" t="s">
-        <v>14</v>
+      <c r="C2" s="3" t="s">
+        <v>12</v>
       </c>
       <c r="D2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" t="s">
         <v>10</v>
       </c>
-      <c r="E2" t="s">
-        <v>9</v>
-      </c>
     </row>
-    <row r="3" spans="1:5" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="5" t="s">
-        <v>12</v>
+      <c r="B3" s="3" t="s">
+        <v>13</v>
       </c>
       <c r="C3" s="2"/>
     </row>
-    <row r="4" spans="1:5" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="C4" s="5"/>
+      <c r="B4" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="2"/>
     </row>
-    <row r="5" spans="1:5" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>7</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C5" s="1"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="C6" s="1"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="7" type="noConversion"/>
+  <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>

</xml_diff>